<commit_message>
Improve web scraping , added regex
</commit_message>
<xml_diff>
--- a/imdb.xlsx
+++ b/imdb.xlsx
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10. Il buono, il brutto, il cattivo</t>
+          <t>10. The Good, the Bad and the Ugly</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22. Shichinin no samurai</t>
+          <t>22. Seven Samurai</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25. Cidade de Deus</t>
+          <t>25. City of God</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26. La vita è bella</t>
+          <t>26. Life Is Beautiful</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -772,36 +772,36 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28. Dune: Part Two</t>
+          <t>28. Terminator 2: Judgment Day</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>paul atreides unites with chani and the fremen while on a warpath of revenge against the conspirators who destroyed his family. facing a choice between the love of his life and the fate of the known universe, he endeavors to prevent a terrible future only he can foresee.—warner bros. pictures</t>
+          <t>over ten years have passed since the first machine called the terminator tried to kill sarah connor and her unborn son, john. the man who will become the future leader of the human resistance against the machines is now a healthy young boy. however, another terminator, called the t-1000, is sent back through time by the supercomputer skynet. this new terminator is more advanced and more powerful than its predecessor and its mission is to kill john connor when he's still a child. however, sarah and john do not have to face the threat of the t-1000 alone. another terminator (identical to the same model that tried and failed to kill sarah connor in 1984) is also sent back through time to protect them. now, the battle for tomorrow has begun.—eric ggg</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29. Terminator 2: Judgment Day</t>
+          <t>29. Star Wars: Episode IV - A New Hope</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>over ten years have passed since the first machine called the terminator tried to kill sarah connor and her unborn son, john. the man who will become the future leader of the human resistance against the machines is now a healthy young boy. however, another terminator, called the t-1000, is sent back through time by the supercomputer skynet. this new terminator is more advanced and more powerful than its predecessor and its mission is to kill john connor when he's still a child. however, sarah and john do not have to face the threat of the t-1000 alone. another terminator (identical to the same model that tried and failed to kill sarah connor in 1984) is also sent back through time to protect them. now, the battle for tomorrow has begun.—eric ggg</t>
+          <t>the imperial forces under orders from cruel darth vader (david prowse) -- hold princess leia (carrie fisher) hostage, in their efforts to quell the rebellion against the galactic empire. luke skywalker (mark hamill) and han solo (harrison ford), captain of the millennium falcon, work together with the companionable droid duo r2-d2 (kenny baker) and c-3po (anthony daniels) to rescue the beautiful princess, help the rebel alliance, and restore freedom and justice to the galaxy.—maschzentertainment</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30. Star Wars</t>
+          <t>30. Dune: Part Two</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>the imperial forces under orders from cruel darth vader (david prowse) -- hold princess leia (carrie fisher) hostage, in their efforts to quell the rebellion against the galactic empire. luke skywalker (mark hamill) and han solo (harrison ford), captain of the millennium falcon, work together with the companionable droid duo r2-d2 (kenny baker) and c-3po (anthony daniels) to rescue the beautiful princess, help the rebel alliance, and restore freedom and justice to the galaxy.—maschzentertainment</t>
+          <t>paul atreides unites with chani and the fremen while on a warpath of revenge against the conspirators who destroyed his family. facing a choice between the love of his life and the fate of the known universe, he endeavors to prevent a terrible future only he can foresee.—warner bros. pictures</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>32. Sen to Chihiro no kamikakushi</t>
+          <t>32. Spirited Away</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>34. Gisaengchung</t>
+          <t>34. Parasite</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -868,24 +868,24 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>36. Spider-Man: Across the Spider-Verse</t>
+          <t>36. Gladiator</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>miles morales returns for the next chapter of the oscar®-winning spider-verse saga, an epic adventure that will transport brooklyn's full-time, friendly neighborhood spider-man across the multiverse to join forces with gwen stacy and a new team of spider-people to face off with a villain more powerful than anything they have ever encountered.—sony pictures</t>
+          <t>maximus is a powerful roman general, loved by the people and the aging emperor, marcus aurelius. before his death, the emperor chooses maximus to be his heir over his own son, commodus, and a power struggle leaves maximus and his family condemned to death. the powerful general is unable to save his family, and his loss of will allows him to get captured and put into the gladiator games until he dies. the only desire that fuels him now is the chance to rise to the top so that he will be able to look into the eyes of the man who will feel his revenge.—chris "morphy" terry</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>37. Gladiator</t>
+          <t>37. Spider-Man: Across the Spider-Verse</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>maximus is a powerful roman general, loved by the people and the aging emperor, marcus aurelius. before his death, the emperor chooses maximus to be his heir over his own son, commodus, and a power struggle leaves maximus and his family condemned to death. the powerful general is unable to save his family, and his loss of will allows him to get captured and put into the gladiator games until he dies. the only desire that fuels him now is the chance to rise to the top so that he will be able to look into the eyes of the man who will feel his revenge.—chris "morphy" terry</t>
+          <t>miles morales returns for the next chapter of the oscar®-winning spider-verse saga, an epic adventure that will transport brooklyn's full-time, friendly neighborhood spider-man across the multiverse to join forces with gwen stacy and a new team of spider-people to face off with a villain more powerful than anything they have ever encountered.—sony pictures</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>40. Léon</t>
+          <t>40. Léon: The Professional</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>44. Hotaru no haka</t>
+          <t>44. Grave of the Fireflies</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>45. Seppuku</t>
+          <t>45. Harakiri</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>48. Intouchables</t>
+          <t>48. The Intouchables</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>49. Nuovo Cinema Paradiso</t>
+          <t>49. Cinema Paradiso</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>52. C'era una volta il West</t>
+          <t>52. Once Upon a Time in the West</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>61. Das Leben der Anderen</t>
+          <t>61. The Lives of Others</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>62. Sunset Blvd.</t>
+          <t>62. Sunset Boulevard</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1324,24 +1324,24 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>74. American Beauty</t>
+          <t>74. Oldboy</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>after his death sometime in his 43rd year, suburbanite lester burnham tells of the last few weeks of his life, during which he had no idea of his imminent passing. he is a husband to real estate agent carolyn burnham and father to high school student jane burnham. although lester and carolyn once loved each other, they now merely tolerate each other. typical wallflower jane also hates both her parents; the three suffer individually in silence in their home life. jane tries to steer clear of both her parents. carolyn, relatively new to the real estate business, wants to create the persona of success to further her career, aspiring to the professional life of buddy kane, the king of the real estate business in their neighborhood. lester merely walks mindlessly through life, including at his job in advertising. his company is downsizing, and he, like all the other employees, has to justify his position to the newly hired efficiency expert to keep his job. things change for lester when he falls in love at first sight with jane's more experienced classmate, angela hayes. both janie and angela can see lester's sexual infatuation with angela, who courts such attention from any man as a sign that she is model material, she having once appeared in seventeen and is a career to which she aspires. lester's infatuation with angela gives him a reenergized view on life, where he openly doesn't care anymore what anyone thinks about what he does, anyone except angela. this infatuation coincides with the fittses moving in next door: homophobic disciplinarian us marine colonel frank fitts who rules the house with a military fist (that fist being both figurative and literal), his semi-comatose wife barbara fitts, and their bright and quietly subversive 18-year-old son ricky fitts, who openly abides by his father's rules while behind the scenes lives by his own quite different perspective. much like lester's infatuation, ricky immediately becomes infatuated with jane; he considers girls like angela as ordinary. the entry of angela and the fittses into the burnhams' lives ultimately leads to each of the players confronting what is truly in his or her heart.—huggo</t>
+          <t>oh dae-su, an obnoxious drunk abducted on a rainy night in 1988, wakes up in a strange, windowless hotel room. kept under lock and key for an unknown reason, oh dae-su's invisible captors keep him fed and systematically sedated to avert suicide, providing only a colour television to keep him company. and after fifteen long years in captivity, perplexed oh dae-su finds himself released. now, his pitiless abductors encourage oh dae-su to track down the ones behind the mysterious kidnapping and finally get his brutal, longed-for revenge on the unknown tormentor. however, who would hate oh dae-su so much that he would deny him a quick and clean death?—nick riganas</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>75. Oldeuboi</t>
+          <t>75. American Beauty</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>oh dae-su, an obnoxious drunk abducted on a rainy night in 1988, wakes up in a strange, windowless hotel room. kept under lock and key for an unknown reason, oh dae-su's invisible captors keep him fed and systematically sedated to avert suicide, providing only a colour television to keep him company. and after fifteen long years in captivity, perplexed oh dae-su finds himself released. now, his pitiless abductors encourage oh dae-su to track down the ones behind the mysterious kidnapping and finally get his brutal, longed-for revenge on the unknown tormentor. however, who would hate oh dae-su so much that he would deny him a quick and clean death?—nick riganas</t>
+          <t>after his death sometime in his 43rd year, suburbanite lester burnham tells of the last few weeks of his life, during which he had no idea of his imminent passing. he is a husband to real estate agent carolyn burnham and father to high school student jane burnham. although lester and carolyn once loved each other, they now merely tolerate each other. typical wallflower jane also hates both her parents; the three suffer individually in silence in their home life. jane tries to steer clear of both her parents. carolyn, relatively new to the real estate business, wants to create the persona of success to further her career, aspiring to the professional life of buddy kane, the king of the real estate business in their neighborhood. lester merely walks mindlessly through life, including at his job in advertising. his company is downsizing, and he, like all the other employees, has to justify his position to the newly hired efficiency expert to keep his job. things change for lester when he falls in love at first sight with jane's more experienced classmate, angela hayes. both janie and angela can see lester's sexual infatuation with angela, who courts such attention from any man as a sign that she is model material, she having once appeared in seventeen and is a career to which she aspires. lester's infatuation with angela gives him a reenergized view on life, where he openly doesn't care anymore what anyone thinks about what he does, anyone except angela. this infatuation coincides with the fittses moving in next door: homophobic disciplinarian us marine colonel frank fitts who rules the house with a military fist (that fist being both figurative and literal), his semi-comatose wife barbara fitts, and their bright and quietly subversive 18-year-old son ricky fitts, who openly abides by his father's rules while behind the scenes lives by his own quite different perspective. much like lester's infatuation, ricky immediately becomes infatuated with jane; he considers girls like angela as ordinary. the entry of angela and the fittses into the burnhams' lives ultimately leads to each of the players confronting what is truly in his or her heart.—huggo</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1420,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>82. Mononoke-hime</t>
+          <t>82. Princess Mononoke</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1444,7 +1444,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>84. Kimi no na wa.</t>
+          <t>84. Your Name.</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>85. Tengoku to jigoku</t>
+          <t>85. High and Low</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>89. Capharnaüm</t>
+          <t>89. Capernaum</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>90. Idi i smotri</t>
+          <t>90. Come and See</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>95. Jagten</t>
+          <t>95. The Hunt</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1600,24 +1600,24 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>97. Oppenheimer</t>
+          <t>97. Reservoir Dogs</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>a dramatization of the life story of j. robert oppenheimer, the physicist who had a large hand in the development of the atomic bomb, thus helping end world war 2. we see his life from university days all the way to post-ww2, where his fame saw him embroiled in political machinations.—grantss</t>
+          <t>six thugs, who are strangers to each other, are hired by a crime boss, joe cabot, to carry out a diamond robbery. right at the outset, they are given false names with the intention that they won't get too close and will concentrate on the job instead. they are completely sure that the robbery is going to be a success. but, when the police show up right at the time and the site of the robbery, panic spreads amongst the group members, and two of them are killed in the subsequent shootout, along with a few policemen and civilians. when the remaining people assemble at the premeditated rendezvous point (a warehouse), they begin to suspect that one of them is an undercover cop.—soumitra</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>98. Reservoir Dogs</t>
+          <t>98. Oppenheimer</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>six thugs, who are strangers to each other, are hired by a crime boss, joe cabot, to carry out a diamond robbery. right at the outset, they are given false names with the intention that they won't get too close and will concentrate on the job instead. they are completely sure that the robbery is going to be a success. but, when the police show up right at the time and the site of the robbery, panic spreads amongst the group members, and two of them are killed in the subsequent shootout, along with a few policemen and civilians. when the remaining people assemble at the premeditated rendezvous point (a warehouse), they begin to suspect that one of them is an undercover cop.—soumitra</t>
+          <t>a dramatization of the life story of j. robert oppenheimer, the physicist who had a large hand in the development of the atomic bomb, thus helping end world war 2. we see his life from university days all the way to post-ww2, where his fame saw him embroiled in political machinations.—grantss</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>105. M - Eine Stadt sucht einen Mörder</t>
+          <t>105. M</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1708,36 +1708,36 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>106. Vertigo</t>
+          <t>106. Scarface</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>following his early retirement as a detective from the san francisco police department, john ferguson - scottie to his friends - becomes obsessed with two women in succession, those obsessions which trouble his long time friend and former fiancée, midge wood, a designer of women's undergarments. the first is wealthy and elegant platinum blonde madeleine elster, the wife of his college acquaintance gavin elster, who hires john to follow her in gavin's belief that she may be a danger to herself in thinking that she has recently been possessed by the spirit of carlotta valdes, madeleine's great-grandmother who she knows nothing about, but who gavin knows committed suicide in being mentally unbalanced when she was twenty-six, madeleine's current age. the second is judy barton, who john spots on the street one day. judy is a working class girl, but what makes john obsessed with her is that, despite her working class style and her brunette hair, she is the spitting image of madeleine, into who he tries to transform judy. the initial question that john has is if there is some connection between madeleine and judy. what happens between john and individually with madeleine and judy is affected by the reason john took that early retirement: a recent workplace incident that showed that he is acrophobic which leads to a severe case of vertigo whenever he looks down from tall heights.—huggo</t>
+          <t>tony montana manages to leave cuba during the mariel exodus of 1980. he finds himself in a florida refugee camp but his friend manny has a way out for them: undertake a contract killing and arrangements will be made to get a green card. he's soon working for drug dealer frank lopez and shows his mettle when a deal with colombian drug dealers goes bad. he also brings a new level of violence to miami. tony is protective of his younger sister but his mother knows what he does for a living and disowns him. tony is impatient and wants it all however, including frank's empire and his mistress elvira hancock. once at the top however, tony's outrageous actions make him a target and everything comes crumbling down.—garykmcd</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>107. Scarface</t>
+          <t>107. Double Indemnity</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>tony montana manages to leave cuba during the mariel exodus of 1980. he finds himself in a florida refugee camp but his friend manny has a way out for them: undertake a contract killing and arrangements will be made to get a green card. he's soon working for drug dealer frank lopez and shows his mettle when a deal with colombian drug dealers goes bad. he also brings a new level of violence to miami. tony is protective of his younger sister but his mother knows what he does for a living and disowns him. tony is impatient and wants it all however, including frank's empire and his mistress elvira hancock. once at the top however, tony's outrageous actions make him a target and everything comes crumbling down.—garykmcd</t>
+          <t>in 1938, walter neff, an experienced salesman of the pacific all risk insurance co., meets the seductive wife of one of his clients, phyllis dietrichson, and they have an affair. phyllis proposes to kill her husband to receive the proceeds of an accident insurance policy and walter devises a scheme to receive twice the amount based on a double indemnity clause. when mr. dietrichson is found dead on a train track, the police accept the determination of accidental death. however, the insurance analyst and walter's best friend barton keyes does not buy the story and suspects that phyllis has murdered her husband with the help of another man.—claudio carvalho, rio de janeiro, brazil</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>108. Double Indemnity</t>
+          <t>108. Vertigo</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>in 1938, walter neff, an experienced salesman of the pacific all risk insurance co., meets the seductive wife of one of his clients, phyllis dietrichson, and they have an affair. phyllis proposes to kill her husband to receive the proceeds of an accident insurance policy and walter devises a scheme to receive twice the amount based on a double indemnity clause. when mr. dietrichson is found dead on a train track, the police accept the determination of accidental death. however, the insurance analyst and walter's best friend barton keyes does not buy the story and suspects that phyllis has murdered her husband with the help of another man.—claudio carvalho, rio de janeiro, brazil</t>
+          <t>following his early retirement as a detective from the san francisco police department, john ferguson - scottie to his friends - becomes obsessed with two women in succession, those obsessions which trouble his long time friend and former fiancée, midge wood, a designer of women's undergarments. the first is wealthy and elegant platinum blonde madeleine elster, the wife of his college acquaintance gavin elster, who hires john to follow her in gavin's belief that she may be a danger to herself in thinking that she has recently been possessed by the spirit of carlotta valdes, madeleine's great-grandmother who she knows nothing about, but who gavin knows committed suicide in being mentally unbalanced when she was twenty-six, madeleine's current age. the second is judy barton, who john spots on the street one day. judy is a working class girl, but what makes john obsessed with her is that, despite her working class style and her brunette hair, she is the spitting image of madeleine, into who he tries to transform judy. the initial question that john has is if there is some connection between madeleine and judy. what happens between john and individually with madeleine and judy is affected by the reason john took that early retirement: a recent workplace incident that showed that he is acrophobic which leads to a severe case of vertigo whenever he looks down from tall heights.—huggo</t>
         </is>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>110. Le fabuleux destin d'Amélie Poulain</t>
+          <t>110. Amélie</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1780,24 +1780,24 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>112. A Clockwork Orange</t>
+          <t>112. Up</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>protagonist alex delarge is an "ultraviolent" youth in futuristic britain. as with all luck, his eventually runs out and he's arrested and convicted of murder. while in prison, alex learns of an experimental program in which convicts are programmed to detest violence. if he goes through the program, his sentence will be reduced and he will be back on the streets sooner than expected. but alex's ordeals are far from over once he hits the streets of britain..—nikki carlyle</t>
+          <t>as a boy, carl fredricksen wanted to explore south america and find the forbidden paradise falls. about 64 years later he gets to begin his journey along with boy scout russell by lifting his house with thousands of balloons. on their journey, they make many new friends including a talking dog, and figure out that someone has evil plans. carl soon realizes that this evildoer is his childhood idol.</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>113. Up</t>
+          <t>113. A Clockwork Orange</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>as a boy, carl fredricksen wanted to explore south america and find the forbidden paradise falls. about 64 years later he gets to begin his journey along with boy scout russell by lifting his house with thousands of balloons. on their journey, they make many new friends including a talking dog, and figure out that someone has evil plans. carl soon realizes that this evildoer is his childhood idol.</t>
+          <t>protagonist alex delarge is an "ultraviolent" youth in futuristic britain. as with all luck, his eventually runs out and he's arrested and convicted of murder. while in prison, alex learns of an experimental program in which convicts are programmed to detest violence. if he goes through the program, his sentence will be reduced and he will be back on the streets sooner than expected. but alex's ordeals are far from over once he hits the streets of britain..—nikki carlyle</t>
         </is>
       </c>
     </row>
@@ -1816,24 +1816,24 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>115. The Sting</t>
+          <t>115. A Separation</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>johnny hooker, a small time grifter, unknowingly steals from doyle lonnegan, a big time crime boss, when he pulls a standard street con. lonnegan demands satisfaction for the insult. after his partner, luther, is killed, hooker flees, and seeks the help of henry gondorff, one of luther's contacts, who is a master of the long con. hooker wants to use gondorff's expertise to take lonnegan for an enormous sum of money to even the score, since he admits he "doesn't know enough about killing to kill him." they devise a complicated scheme and amass a talented group of other con artists who want their share of the reparations. the stakes are high in this game, and our heroes must not only deal with lonnegan's murderous tendencies, but also other side players who want a piece of the action. to win, hooker and gondorff will need all their skills...and a fair amount of confidence.—headlessannie</t>
+          <t>nader (payman maadi) and simin (leila hatami) argue about living abroad. simin prefers to live abroad to provide better opportunities for their only daughter, termeh. however, nader refuses to go because he thinks he must stay in iran and take care of his father (ali-asghar shahbazi), who suffers from alzheimers. however, simin is determined to get a divorce and leave the country with her daughter.—amin davoodi</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>116. Jodaeiye Nader az Simin</t>
+          <t>116. The Sting</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>nader (payman maadi) and simin (leila hatami) argue about living abroad. simin prefers to live abroad to provide better opportunities for their only daughter, termeh. however, nader refuses to go because he thinks he must stay in iran and take care of his father (ali-asghar shahbazi), who suffers from alzheimers. however, simin is determined to get a divorce and leave the country with her daughter.—amin davoodi</t>
+          <t>johnny hooker, a small time grifter, unknowingly steals from doyle lonnegan, a big time crime boss, when he pulls a standard street con. lonnegan demands satisfaction for the insult. after his partner, luther, is killed, hooker flees, and seeks the help of henry gondorff, one of luther's contacts, who is a master of the long con. hooker wants to use gondorff's expertise to take lonnegan for an enormous sum of money to even the score, since he admits he "doesn't know enough about killing to kill him." they devise a complicated scheme and amass a talented group of other con artists who want their share of the reparations. the stakes are high in this game, and our heroes must not only deal with lonnegan's murderous tendencies, but also other side players who want a piece of the action. to win, hooker and gondorff will need all their skills...and a fair amount of confidence.—headlessannie</t>
         </is>
       </c>
     </row>
@@ -1864,24 +1864,24 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>119. Metropolis</t>
+          <t>119. Like Stars on Earth</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>sometime in the future, the city of metropolis is home to a utopian society where its wealthy residents live a carefree life. one of those is freder fredersen. one day, he spots a beautiful woman with a group of children, she and the children quickly disappear. trying to follow her, he is horrified to find an underground world of workers who apparently run the machinery that keeps the utopian world above ground functioning. one of the few people above ground who knows about the world below is freder's father, john fredersen, who is the founder and master of metropolis. freder learns that the woman is called maria, who espouses the need to join the "hands" - the workers - to the "head" - those in power above - by a mediator who will act as the "heart". freder wants to help the plight of the workers in their struggle for a better life. but when john learns of what maria is advocating and that freder has joined their cause, with the assistance of an old colleague. an inventor called rotwang, who turns out to be but their nemesis goes to works towards quashing a proposed uprising, with maria at the centre of their plan. john, unaware that rotwang has his own agenda., makes plans that include shutting down the machines, with the prospect of unleashing total anarchy both above and below ground.—huggo</t>
+          <t>ishaan awasthi is an eight-year-old child whose world is filled with wonders that no one else seems to appretiate are just not important in the world of adults, who are much more interested in things like homework, marks and neatness. and ishaan just cannot seem to get anything right in class. when he gets into far more trouble than his parents can handle, he is packed off to a boarding school to 'be disciplined'. things are no different at his new school, and ishaan has to contend with the added trauma of separation from his family. one day a new art teacher bursts onto the scene, ram shankar nikumbh, who infects the students with joy and optimism. he breaks all the rules of 'how things are done' by asking them to think, dream and imagine, and all the children respond with enthusiasm, all except ishaan. nikumbh soon realizes that ishaan is very unhappy, and he sets out to discover why. with time, patience and care, he ultimately helps ishaan find himself.</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>120. Taare Zameen Par</t>
+          <t>120. Metropolis</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>ishaan awasthi is an eight-year-old child whose world is filled with wonders that no one else seems to appretiate are just not important in the world of adults, who are much more interested in things like homework, marks and neatness. and ishaan just cannot seem to get anything right in class. when he gets into far more trouble than his parents can handle, he is packed off to a boarding school to 'be disciplined'. things are no different at his new school, and ishaan has to contend with the added trauma of separation from his family. one day a new art teacher bursts onto the scene, ram shankar nikumbh, who infects the students with joy and optimism. he breaks all the rules of 'how things are done' by asking them to think, dream and imagine, and all the children respond with enthusiasm, all except ishaan. nikumbh soon realizes that ishaan is very unhappy, and he sets out to discover why. with time, patience and care, he ultimately helps ishaan find himself.</t>
+          <t>sometime in the future, the city of metropolis is home to a utopian society where its wealthy residents live a carefree life. one of those is freder fredersen. one day, he spots a beautiful woman with a group of children, she and the children quickly disappear. trying to follow her, he is horrified to find an underground world of workers who apparently run the machinery that keeps the utopian world above ground functioning. one of the few people above ground who knows about the world below is freder's father, john fredersen, who is the founder and master of metropolis. freder learns that the woman is called maria, who espouses the need to join the "hands" - the workers - to the "head" - those in power above - by a mediator who will act as the "heart". freder wants to help the plight of the workers in their struggle for a better life. but when john learns of what maria is advocating and that freder has joined their cause, with the assistance of an old colleague. an inventor called rotwang, who turns out to be but their nemesis goes to works towards quashing a proposed uprising, with maria at the centre of their plan. john, unaware that rotwang has his own agenda., makes plans that include shutting down the machines, with the prospect of unleashing total anarchy both above and below ground.—huggo</t>
         </is>
       </c>
     </row>
@@ -1900,43 +1900,43 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>122. Hamilton</t>
+          <t>122. L.A. Confidential</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>"hamilton" is the story of america then, told by america now. featuring a score that blends hip-hop, jazz, r&amp;b, and show tunes, "hamilton" has taken the story of american founding father alexander hamilton and created a revolutionary moment in theater--a musical that has had a profound impact on culture, politics, and education. captured at the richard rodgers theater on broadway in june 2016, the film transports its audience into the world of the broadway show in a uniquely intimate way.—the walt disney studios</t>
+          <t>1950's los angeles is the seedy backdrop for this intricate noir-ish tale of police corruption and hollywood sleaze. three very different cops are all after the truth, each in their own style: ed exley, the golden boy of the police force, willing to do almost anything to get ahead, except sell out; bud white, ready to break the rules to seek justice, but barely able to keep his raging violence under control; and jack vincennes, always looking for celebrity and a quick buck until his conscience drives him to join exley and white down the one-way path to find the truth behind the dark world of l.a. crime.—greg bole &lt;bole@life.bio.sunysb.edu&gt;</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>123. L.A. Confidential</t>
+          <t>123. 1917</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>1950's los angeles is the seedy backdrop for this intricate noir-ish tale of police corruption and hollywood sleaze. three very different cops are all after the truth, each in their own style: ed exley, the golden boy of the police force, willing to do almost anything to get ahead, except sell out; bud white, ready to break the rules to seek justice, but barely able to keep his raging violence under control; and jack vincennes, always looking for celebrity and a quick buck until his conscience drives him to join exley and white down the one-way path to find the truth behind the dark world of l.a. crime.—greg bole &lt;bole@life.bio.sunysb.edu&gt;</t>
+          <t>april 1917, the western front. two british soldiers are sent to deliver an urgent message to an isolated regiment. if the message is not received in time the regiment will walk into a trap and be massacred. to get to the regiment they will need to cross through enemy territory. time is of the essence and the journey will be fraught with danger.—grantss</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>124. 1917</t>
+          <t>124. Hamilton</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>april 1917, the western front. two british soldiers are sent to deliver an urgent message to an isolated regiment. if the message is not received in time the regiment will walk into a trap and be massacred. to get to the regiment they will need to cross through enemy territory. time is of the essence and the journey will be fraught with danger.—grantss</t>
+          <t>"hamilton" is the story of america then, told by america now. featuring a score that blends hip-hop, jazz, r&amp;b, and show tunes, "hamilton" has taken the story of american founding father alexander hamilton and created a revolutionary moment in theater--a musical that has had a profound impact on culture, politics, and education. captured at the richard rodgers theater on broadway in june 2016, the film transports its audience into the world of the broadway show in a uniquely intimate way.—the walt disney studios</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>125. Ladri di biciclette</t>
+          <t>125. Bicycle Thieves</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -1960,7 +1960,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>127. Der Untergang</t>
+          <t>127. Downfall</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -1984,7 +1984,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>129. Per qualche dollaro in più</t>
+          <t>129. For a Few Dollars More</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2188,7 +2188,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>146. El laberinto del fauno</t>
+          <t>146. Pan's Labyrinth</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>153. Yôjinbô</t>
+          <t>153. Yojimbo</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -2332,24 +2332,24 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>158. Rashômon</t>
+          <t>158. Howl's Moving Castle</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>a priest, a woodcutter and another man are taking refuge from a rainstorm in the shell of a former gatehouse called rashômon. the priest and the woodcutter are recounting the story of a murdered samurai whose body the woodcutter discovered three days earlier in a forest grove. both were summoned to testify at the murder trial, the priest who ran into the samurai and his wife traveling through the forest just before the murder occurred. three other people who testified at the trial are supposedly the only direct witnesses: a notorious bandit named tajômaru, who allegedly murdered the samurai and raped his wife; the white veil cloaked wife of the samurai; and the samurai himself who testifies through the use of a medium. the three tell a similarly structured story - that tajômaru kidnapped and bound the samurai so that he could rape the wife - but which ultimately contradict each other, the motivations and the actual killing being what differ. the woodcutter reveals at rashômon that he knows more than he let on at the trial, thus bringing into question his own actions. but another discovery at rashômon and the resulting actions from the discovery bring back into focus the woodcutter's own humanity or lack thereof.—huggo</t>
+          <t>with her country's peace constantly under threat, sophie, a lively but unloved milliner, catches the attention of an unexpected defender. but as the wide-eyed damsel in distress crosses paths with handsome howl, a talented young magician with excess emotional baggage, a fit of jealousy turns the hat maker's world upside down forever. now, stained by the indelible mark of the wicked witch of the waste, sophie must move mountains to break the pitiless spell, including facing her fears and the mysterious sorcerer. however, has anyone ever set foot in howl's impenetrable home, a walking wonder powered by a fiery heart, and lived to tell the tale?—nick riganas</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>159. Hauru no ugoku shiro</t>
+          <t>159. Rashomon</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>with her country's peace constantly under threat, sophie, a lively but unloved milliner, catches the attention of an unexpected defender. but as the wide-eyed damsel in distress crosses paths with handsome howl, a talented young magician with excess emotional baggage, a fit of jealousy turns the hat maker's world upside down forever. now, stained by the indelible mark of the wicked witch of the waste, sophie must move mountains to break the pitiless spell, including facing her fears and the mysterious sorcerer. however, has anyone ever set foot in howl's impenetrable home, a walking wonder powered by a fiery heart, and lived to tell the tale?—nick riganas</t>
+          <t>a priest, a woodcutter and another man are taking refuge from a rainstorm in the shell of a former gatehouse called rashômon. the priest and the woodcutter are recounting the story of a murdered samurai whose body the woodcutter discovered three days earlier in a forest grove. both were summoned to testify at the murder trial, the priest who ran into the samurai and his wife traveling through the forest just before the murder occurred. three other people who testified at the trial are supposedly the only direct witnesses: a notorious bandit named tajômaru, who allegedly murdered the samurai and raped his wife; the white veil cloaked wife of the samurai; and the samurai himself who testifies through the use of a medium. the three tell a similarly structured story - that tajômaru kidnapped and bound the samurai so that he could rape the wife - but which ultimately contradict each other, the motivations and the actual killing being what differ. the woodcutter reveals at rashômon that he knows more than he let on at the trial, thus bringing into question his own actions. but another discovery at rashômon and the resulting actions from the discovery bring back into focus the woodcutter's own humanity or lack thereof.—huggo</t>
         </is>
       </c>
     </row>
@@ -2368,24 +2368,24 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>161. Chinatown</t>
+          <t>161. Dial M for Murder</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>in 1937 los angeles, private investigator jake 'j.j.' gittes specializes in cheating-spouse cases. his current target is hollis mulwray, high-profile chief engineer for the los angeles department of water and power, whose wife suspects him of infidelity. in following mulwray, gittes witnesses some usual business dealings, such as a public meeting for construction of a new dam to create additional water supply for los angeles, as fresh water is vital to the growing community during the chronic drought; mulwray opposes the dam. eventually gittes sees mulwray meeting with an unknown young woman who isn't his wife. once news of the supposed tryst between mulwray and this woman hits the media, additional information comes to light that makes gittes believe that mulwray is being framed for something and that he himself is being set up. in his investigation of the issue behind mulwray's framing and his own setup, gittes is assisted by mulwray's wife evelyn, but he thinks she isn't being forthright with him. the further he gets into the investigation, the more secrets he uncovers about the mulwrays' professional and personal dealings, including mulwray's former business-partnership with evelyn's father, noah cross. the identity of the unknown woman may be the key to uncovering the whole story.—huggo</t>
+          <t>in london, wealthy margot mary wendice had a brief love affair with the american writer mark halliday while her husband and professional tennis player tony wendice was on a tennis tour. tony quits playing to dedicate to his wife and finds a regular job. she decides to give him a second chance for their marriage. when mark arrives from america to visit the couple, margot tells him that she had destroyed all his letters but one that was stolen. subsequently she was blackmailed, but she had never retrieved the stolen letter. tony arrives home, claims that he needs to work and asks margot to go with mark to the theater. meanwhile tony calls captain lesgate (aka charles alexander swann who studied with him at college) and blackmails him to murder his wife, so that he can inherit her fortune. but there is no perfect crime, and things do not work as planned.—claudio carvalho, rio de janeiro, brazil</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>162. Dial M for Murder</t>
+          <t>162. Chinatown</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>in london, wealthy margot mary wendice had a brief love affair with the american writer mark halliday while her husband and professional tennis player tony wendice was on a tennis tour. tony quits playing to dedicate to his wife and finds a regular job. she decides to give him a second chance for their marriage. when mark arrives from america to visit the couple, margot tells him that she had destroyed all his letters but one that was stolen. subsequently she was blackmailed, but she had never retrieved the stolen letter. tony arrives home, claims that he needs to work and asks margot to go with mark to the theater. meanwhile tony calls captain lesgate (aka charles alexander swann who studied with him at college) and blackmails him to murder his wife, so that he can inherit her fortune. but there is no perfect crime, and things do not work as planned.—claudio carvalho, rio de janeiro, brazil</t>
+          <t>in 1937 los angeles, private investigator jake 'j.j.' gittes specializes in cheating-spouse cases. his current target is hollis mulwray, high-profile chief engineer for the los angeles department of water and power, whose wife suspects him of infidelity. in following mulwray, gittes witnesses some usual business dealings, such as a public meeting for construction of a new dam to create additional water supply for los angeles, as fresh water is vital to the growing community during the chronic drought; mulwray opposes the dam. eventually gittes sees mulwray meeting with an unknown young woman who isn't his wife. once news of the supposed tryst between mulwray and this woman hits the media, additional information comes to light that makes gittes believe that mulwray is being framed for something and that he himself is being set up. in his investigation of the issue behind mulwray's framing and his own setup, gittes is assisted by mulwray's wife evelyn, but he thinks she isn't being forthright with him. the further he gets into the investigation, the more secrets he uncovers about the mulwrays' professional and personal dealings, including mulwray's former business-partnership with evelyn's father, noah cross. the identity of the unknown woman may be the key to uncovering the whole story.—huggo</t>
         </is>
       </c>
     </row>
@@ -2404,31 +2404,31 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>164. V for Vendetta</t>
+          <t>164. Lock, Stock and Two Smoking Barrels</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>in the distant future, evey hammond is an average citizen of the united kingdom, which is under the rule of the fascist and tyrannical norsefire party. she is an employee of the state-run british television network, but soon, she becomes the number one enemy of the state together with an enigmatic and larger-than-life freedom fighter known only by the letter "v". v informs evey that she must hide in his underground lair for at least one year, and while she is reluctant to the idea at first, a bond soon forms between the two individuals. in the meanwhile, the mysterious past of v is gradually revealed to the police inspector tasked with capturing him, eric finch, and it is not long until he starts questioning everything his government stands for.—goddangwatir</t>
+          <t>four jack-the-lads find themselves heavily - seriously heavily - in debt to an east end hard man and his enforcers after a crooked card game. overhearing their neighbours in the next flat plotting to hold up a group of out-of-their-depth drug growers, our heroes decide to stitch up the robbers in turn. in a way the confusion really starts when a pair of antique double-barrelled shotguns go missing in a completely different scam.</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>165. Lock, Stock and Two Smoking Barrels</t>
+          <t>165. V for Vendetta</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>four jack-the-lads find themselves heavily - seriously heavily - in debt to an east end hard man and his enforcers after a crooked card game. overhearing their neighbours in the next flat plotting to hold up a group of out-of-their-depth drug growers, our heroes decide to stitch up the robbers in turn. in a way the confusion really starts when a pair of antique double-barrelled shotguns go missing in a completely different scam.</t>
+          <t>in the distant future, evey hammond is an average citizen of the united kingdom, which is under the rule of the fascist and tyrannical norsefire party. she is an employee of the state-run british television network, but soon, she becomes the number one enemy of the state together with an enigmatic and larger-than-life freedom fighter known only by the letter "v". v informs evey that she must hide in his underground lair for at least one year, and while she is reluctant to the idea at first, a bond soon forms between the two individuals. in the meanwhile, the mysterious past of v is gradually revealed to the police inspector tasked with capturing him, eric finch, and it is not long until he starts questioning everything his government stands for.—goddangwatir</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>166. El secreto de sus ojos</t>
+          <t>166. The Secret in Their Eyes</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2572,31 +2572,31 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>178. Tonari no Totoro</t>
+          <t>178. Million Dollar Baby</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>excited about reuniting with their ailing mother, close-knit sisters satsuki and mei embark on an exciting adventure when they move with their loving professor father to a new house in the verdant countryside of 1950s summer japan. now, nothing can stop them. and with mum in the hospital, the girls have all the time in the world to explore nature and the dense adjacent forest, the home of bashful mystical creatures only children can see. under the clear blue sky's cloudless bliss and the bright yellow sun's promise of a luminous future, nothing can blemish the young sisters' flawless fantasy--not even life's trying times. after all, mother is getting better. then, one radiant morning, as the shimmering green leaves of the towering camphor trees swayed in the soft morning breeze, the wide-eyed siblings stumbled upon a totoro. but who is the enchanting visitor? will the rotund neighbour, with his fluffy fur and mysterious eyes, be the girls' forever friend?—nick riganas</t>
+          <t>wanting to learn from the best, aspiring boxer maggie fitzgerald (hilary swank) wants frankie dunn (clint eastwood) to train her. at the outset, he flatly refuses saying he has no interest in training a girl. frankie leads a lonely existence, alienated from his only daughter and having few friends. maggie's rough around the edges, but shows a lot of grit in the ring and he eventually relents. maggie not only proves to be the boxer he always dreamed of having under his wing, but a friend who fills the great void he's had in his life. maggie's career skyrockets, but an accident in the ring leads her to ask frankie for one last favor.—garykmcd</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>179. Million Dollar Baby</t>
+          <t>179. My Neighbor Totoro</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>wanting to learn from the best, aspiring boxer maggie fitzgerald (hilary swank) wants frankie dunn (clint eastwood) to train her. at the outset, he flatly refuses saying he has no interest in training a girl. frankie leads a lonely existence, alienated from his only daughter and having few friends. maggie's rough around the edges, but shows a lot of grit in the ring and he eventually relents. maggie not only proves to be the boxer he always dreamed of having under his wing, but a friend who fills the great void he's had in his life. maggie's career skyrockets, but an accident in the ring leads her to ask frankie for one last favor.—garykmcd</t>
+          <t>excited about reuniting with their ailing mother, close-knit sisters satsuki and mei embark on an exciting adventure when they move with their loving professor father to a new house in the verdant countryside of 1950s summer japan. now, nothing can stop them. and with mum in the hospital, the girls have all the time in the world to explore nature and the dense adjacent forest, the home of bashful mystical creatures only children can see. under the clear blue sky's cloudless bliss and the bright yellow sun's promise of a luminous future, nothing can blemish the young sisters' flawless fantasy--not even life's trying times. after all, mother is getting better. then, one radiant morning, as the shimmering green leaves of the towering camphor trees swayed in the soft morning breeze, the wide-eyed siblings stumbled upon a totoro. but who is the enchanting visitor? will the rotund neighbour, with his fluffy fur and mysterious eyes, be the girls' forever friend?—nick riganas</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>180. Harry Potter and the Deathly Hallows - Part 2</t>
+          <t>180. Harry Potter and the Deathly Hallows: Part 2</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -2608,7 +2608,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>181. Bacheha-Ye aseman</t>
+          <t>181. Children of Heaven</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -2644,48 +2644,48 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>184. Before Sunrise</t>
+          <t>184. Ben-Hur</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>american tourist jesse and french student celine meet by chance on the train from budapest to vienna. sensing that they are developing a connection, jesse asks celine to spend the day with him in vienna, and she agrees. so they pass the time before his scheduled flight the next morning together. how do two perfect strangers connect so intimately over the course of a single day? what is that special thing that bonds two people so strongly? as their bond turns to love, what will happen to them the next morning when jesse flies away?—randywong70@comcast.net</t>
+          <t>judah ben-hur lives as a rich jewish prince and merchant in jerusalem at the beginning of the 1st century. together with the new governor his old friend messala arrives as commanding officer of the roman legions. at first they are happy to meet after a long time but their different politic views separate them. during the welcome parade a roof tile falls down from judah's house and injures the governor. although messala knows they are not guilty, he sends judah to the galleys and throws his mother and sister into prison. but judah swears to come back and take revenge.—matthias scheler &lt;tron@lyssa.owl.de&gt;</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>185. Ben-Hur</t>
+          <t>185. Before Sunrise</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>judah ben-hur lives as a rich jewish prince and merchant in jerusalem at the beginning of the 1st century. together with the new governor his old friend messala arrives as commanding officer of the roman legions. at first they are happy to meet after a long time but their different politic views separate them. during the welcome parade a roof tile falls down from judah's house and injures the governor. although messala knows they are not guilty, he sends judah to the galleys and throws his mother and sister into prison. but judah swears to come back and take revenge.—matthias scheler &lt;tron@lyssa.owl.de&gt;</t>
+          <t>american tourist jesse and french student celine meet by chance on the train from budapest to vienna. sensing that they are developing a connection, jesse asks celine to spend the day with him in vienna, and she agrees. so they pass the time before his scheduled flight the next morning together. how do two perfect strangers connect so intimately over the course of a single day? what is that special thing that bonds two people so strongly? as their bond turns to love, what will happen to them the next morning when jesse flies away?—randywong70@comcast.net</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>186. Barry Lyndon</t>
+          <t>186. The Grand Budapest Hotel</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>in the eighteenth century, in a small village in ireland, redmond barry (ryan o'neal) is a young farm boy in love with his cousin nora brady (gay hamilton). when nora gets engaged to british captain john quin (leonard rossiter), barry challenges him to a duel of pistols. he wins and escapes to dublin, but is robbed on the road. without an alternative, barry joins the british army to fight in the seven years war. he deserts and is forced to join the prussian army, where he saves the life of his captain and becomes his protégé and spy of irish gambler chevalier de balibari (patrick magee). he helps chevalier and becomes his associate until he decides to marry the wealthy lady lyndon (marisa berenson). they move to england and barry, in his obsession of nobility, dissipates her fortune and makes a dangerous and revengeful enemy.—claudio carvalho, rio de janeiro, brazil</t>
+          <t>this movie recounts the adventures of m. gustave, a legendary concierge at a famous european hotel between the wars, and zero moustafa, the lobby boy who becomes his most trusted friend. the story involves the theft and recovery of a priceless renaissance painting and the battle for an enormous family fortune - all against the backdrop of a suddenly and dramatically changing continent.—fox searchlight pictures</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>187. The Grand Budapest Hotel</t>
+          <t>187. Barry Lyndon</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>this movie recounts the adventures of m. gustave, a legendary concierge at a famous european hotel between the wars, and zero moustafa, the lobby boy who becomes his most trusted friend. the story involves the theft and recovery of a priceless renaissance painting and the battle for an enormous family fortune - all against the backdrop of a suddenly and dramatically changing continent.—fox searchlight pictures</t>
+          <t>in the eighteenth century, in a small village in ireland, redmond barry (ryan o'neal) is a young farm boy in love with his cousin nora brady (gay hamilton). when nora gets engaged to british captain john quin (leonard rossiter), barry challenges him to a duel of pistols. he wins and escapes to dublin, but is robbed on the road. without an alternative, barry joins the british army to fight in the seven years war. he deserts and is forced to join the prussian army, where he saves the life of his captain and becomes his protégé and spy of irish gambler chevalier de balibari (patrick magee). he helps chevalier and becomes his associate until he decides to marry the wealthy lady lyndon (marisa berenson). they move to england and barry, in his obsession of nobility, dissipates her fortune and makes a dangerous and revengeful enemy.—claudio carvalho, rio de janeiro, brazil</t>
         </is>
       </c>
     </row>
@@ -2716,67 +2716,67 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>190. The Gold Rush</t>
+          <t>190. Mad Max: Fury Road</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>a lone prospector ventures into alaska looking for gold. he gets mixed up with some burly characters and falls in love with the beautiful georgia. he tries to win her heart with his singular charm.—john j. magee &lt;magee@helix.mgh.harvard.edu&gt;</t>
+          <t>an apocalyptic story set in the furthest reaches of our planet, in a stark desert landscape where humanity is broken, and almost everyone is crazed fighting for the necessities of life. within this world exist two rebels on the run who just might be able to restore order. there's max, a man of action and a man of few words, who seeks peace of mind following the loss of his wife and child in the aftermath of the chaos. and furiosa, a woman of action and a woman who believes her path to survival may be achieved if she can make it across the desert back to her childhood homeland.—production</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>191. Salinui chueok</t>
+          <t>191. The Gold Rush</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>1986. in a rural district of south korea, two women have been recently raped and murdered. working on the case are detectives park doo-man and cho yong-koo. their efforts are impeded by some sloppy crime scene procedure by the police. their methods of solving cases are also quite basic, essentially amounting to beating confessions out of suspects. all this leads to nothing and the police chief brings in a more sophisticated and intelligent detective from seoul, seo tae-yoon. with his arrival the methods improve but they still don't have the killer. then another woman is found murdered and a pattern emerges.—grantss</t>
+          <t>a lone prospector ventures into alaska looking for gold. he gets mixed up with some burly characters and falls in love with the beautiful georgia. he tries to win her heart with his singular charm.—john j. magee &lt;magee@helix.mgh.harvard.edu&gt;</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>192. In the Name of the Father</t>
+          <t>192. Dead Poets Society</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>young belfastian gerry conlon (daniel day-lewis) admits that he was in london at the time of the incident. he also admits that he is not a model citizen, having committed a petty robbery while in london. he does however profess his innocence when it comes to the bombing of the guildford pub in london in 1974, the event which killed several people inside. a self-professed non-political person, he and his three co-accused, dubbed the guildford four, are thought to be provisional members of the i.r.a. their self-professed innocence is despite each having signed a statement of guilt which they claim were signed under duress. their case includes having provable alibis for the time frame of the bombing. and eventually, joe mcandrew (don baker), a known i.r.a. member, admits to the bombing. dubbed the maguire seven, seven others, primarily members of gerry's extended family including his father giuseppe (pete postlethwaite), are accused of being accessories to the bombing. following on the work initiated by giuseppe, gerry works on a campaign to prove their collective innocence, this work with the assistance of compassionate lawyer gareth peirce (dame emma thompson). as gareth works on this campaign, she is faced with obstacle after obstacle placed by robert dixon (corin redgrave), who led the initial investigation and questioning of the four accused on behalf of the police.—huggo</t>
+          <t>painfully shy todd anderson has been sent to the school where his popular older brother was valedictorian. his roommate, neil perry, although exceedingly bright and popular, is very much under the thumb of his overbearing father. the two, along with their other friends, meet professor keating, their new english teacher, who tells them of the dead poets society, and encourages them to go against the status quo. each does so in his own way, and is changed for life.—liz jordan &lt;c9310494@alinga.newcastle.edu.au&gt;</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>193. Dead Poets Society</t>
+          <t>193. Memories of Murder</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>painfully shy todd anderson has been sent to the school where his popular older brother was valedictorian. his roommate, neil perry, although exceedingly bright and popular, is very much under the thumb of his overbearing father. the two, along with their other friends, meet professor keating, their new english teacher, who tells them of the dead poets society, and encourages them to go against the status quo. each does so in his own way, and is changed for life.—liz jordan &lt;c9310494@alinga.newcastle.edu.au&gt;</t>
+          <t>1986. in a rural district of south korea, two women have been recently raped and murdered. working on the case are detectives park doo-man and cho yong-koo. their efforts are impeded by some sloppy crime scene procedure by the police. their methods of solving cases are also quite basic, essentially amounting to beating confessions out of suspects. all this leads to nothing and the police chief brings in a more sophisticated and intelligent detective from seoul, seo tae-yoon. with his arrival the methods improve but they still don't have the killer. then another woman is found murdered and a pattern emerges.—grantss</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>194. Mad Max: Fury Road</t>
+          <t>194. In the Name of the Father</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>an apocalyptic story set in the furthest reaches of our planet, in a stark desert landscape where humanity is broken, and almost everyone is crazed fighting for the necessities of life. within this world exist two rebels on the run who just might be able to restore order. there's max, a man of action and a man of few words, who seeks peace of mind following the loss of his wife and child in the aftermath of the chaos. and furiosa, a woman of action and a woman who believes her path to survival may be achieved if she can make it across the desert back to her childhood homeland.—production</t>
+          <t>young belfastian gerry conlon (daniel day-lewis) admits that he was in london at the time of the incident. he also admits that he is not a model citizen, having committed a petty robbery while in london. he does however profess his innocence when it comes to the bombing of the guildford pub in london in 1974, the event which killed several people inside. a self-professed non-political person, he and his three co-accused, dubbed the guildford four, are thought to be provisional members of the i.r.a. their self-professed innocence is despite each having signed a statement of guilt which they claim were signed under duress. their case includes having provable alibis for the time frame of the bombing. and eventually, joe mcandrew (don baker), a known i.r.a. member, admits to the bombing. dubbed the maguire seven, seven others, primarily members of gerry's extended family including his father giuseppe (pete postlethwaite), are accused of being accessories to the bombing. following on the work initiated by giuseppe, gerry works on a campaign to prove their collective innocence, this work with the assistance of compassionate lawyer gareth peirce (dame emma thompson). as gareth works on this campaign, she is faced with obstacle after obstacle placed by robert dixon (corin redgrave), who led the initial investigation and questioning of the four accused on behalf of the police.—huggo</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>195. Relatos salvajes</t>
+          <t>195. Wild Tales</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -2848,24 +2848,24 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>201. Jaws</t>
+          <t>201. How to Train Your Dragon</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>it's a hot summer on amity island, a small community whose main business is its beaches. when new sheriff martin brody discovers the remains of a shark attack victim, his first inclination is to close the beaches to swimmers. this doesn't sit well with mayor larry vaughn and several of the local businessmen. brody backs down to his regret as that weekend a young boy is killed by the predator. the dead boy's mother puts out a bounty on the shark and amity is soon swamped with amateur hunters and fisherman hoping to cash in on the reward. a local fisherman with much experience hunting sharks, quint, offers to hunt down the creature for a hefty fee. soon quint, brody and matt hooper from the oceanographic institute are at sea hunting the great white shark. as brody succinctly surmises after their first encounter with the creature, they're going to need a bigger boat.—garykmcd</t>
+          <t>long ago up north on the island of berk, the young viking, hiccup, wants to join his town's fight against the dragons that continually raid their town. however, his macho father and village leader, stoik the vast, will not allow his small, clumsy, but inventive son to do so. regardless, hiccup ventures out into battle and downs a mysterious night fury dragon with his invention, but can't bring himself to kill it. instead, hiccup and the dragon, whom he dubs toothless, begin a friendship that would open up both their worlds as the observant boy learns that his people have misjudged the species. but even as the two each take flight in their own way, they find that they must fight the destructive ignorance plaguing their world.—kenneth chisholm (kchishol@rogers.com)</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>202. How to Train Your Dragon</t>
+          <t>202. Jaws</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>long ago up north on the island of berk, the young viking, hiccup, wants to join his town's fight against the dragons that continually raid their town. however, his macho father and village leader, stoik the vast, will not allow his small, clumsy, but inventive son to do so. regardless, hiccup ventures out into battle and downs a mysterious night fury dragon with his invention, but can't bring himself to kill it. instead, hiccup and the dragon, whom he dubs toothless, begin a friendship that would open up both their worlds as the observant boy learns that his people have misjudged the species. but even as the two each take flight in their own way, they find that they must fight the destructive ignorance plaguing their world.—kenneth chisholm (kchishol@rogers.com)</t>
+          <t>it's a hot summer on amity island, a small community whose main business is its beaches. when new sheriff martin brody discovers the remains of a shark attack victim, his first inclination is to close the beaches to swimmers. this doesn't sit well with mayor larry vaughn and several of the local businessmen. brody backs down to his regret as that weekend a young boy is killed by the predator. the dead boy's mother puts out a bounty on the shark and amity is soon swamped with amateur hunters and fisherman hoping to cash in on the reward. a local fisherman with much experience hunting sharks, quint, offers to hunt down the creature for a hefty fee. soon quint, brody and matt hooper from the oceanographic institute are at sea hunting the great white shark. as brody succinctly surmises after their first encounter with the creature, they're going to need a bigger boat.—garykmcd</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>204. Le salaire de la peur</t>
+          <t>204. The Wages of Fear</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -2896,7 +2896,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>205. Mary and Max.</t>
+          <t>205. Mary and Max</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -2908,7 +2908,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>206. Smultronstället</t>
+          <t>206. Wild Strawberries</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -2949,14 +2949,14 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>as enzo ferrari's fast rosso-corsa racing cars dominate the mid-1960s motorsport world, the american car designer, carroll shelby, is forced to retire after winning the demanding 1959 '24 hours of le mans' endurance race. but, before long, an unexpected proposition by the vice president of henry ford's motor company, lee iacocca, will offer an opportunity to beat the italians at their own game. now, under those pressing circumstances, the british sports car driver and racing engineer, ken miles, reluctantly agrees to lend a hand and improve the firm's image, as ford's race team has less than ninety days to rewrite history. as a result, the non-conformist duo comes up with the mighty ford gt40 mk i high-performance racing car. can shelby and miles break ferrari's streak?—nick riganas</t>
+          <t>in the mid-1960s, enzo ferrari's fast rosso-corsa racing cars were dominating the motorsport world. meanwhile, carroll shelby, an american car designer, had retired after winning the demanding 1959 '24 hours of le mans' endurance race. however, an unexpected proposition from lee iacocca, the vice president of henry ford's motor company, presented an opportunity to beat the italians at their own game. under these pressing circumstances, ken miles, a british sports car driver and racing engineer, reluctantly agreed to help improve the americans' image. but ford's race team had less than ninety days to rewrite history. as a result, the non-conformist duo came up with the ford gt40 mk i, a powerful, high-performance racing car. nevertheless, the question remained. can shelby and miles break ferrari's long winning streak?—nick riganas</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>210. Tôkyô monogatari</t>
+          <t>210. Tokyo Story</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -2992,7 +2992,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>213. Det sjunde inseglet</t>
+          <t>213. The Seventh Seal</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -3076,7 +3076,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>220. La passion de Jeanne d'Arc</t>
+          <t>220. The Passion of Joan of Arc</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -3148,24 +3148,24 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>226. Rush</t>
+          <t>226. Jai Bhim</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>set against the sexy, glamorous golden age of formula 1 racing in the 1970s, the film is based on the true story of a great sporting rivalry between handsome english playboy james hunt (hemsworth), and his methodical, brilliant opponent, austrian driver niki lauda (bruhl). the story follows their distinctly-different personal styles on and off the track, their loves, and the astonishing 1976 season in which both drivers were willing to risk everything to become world champion in a sport with no margin for error: if you make a mistake, you die.—p. morgan</t>
+          <t>rajakannu and his wife sengeni belong to a lower cast and works as labors in the field to protect it from rats thou they live life of poverty but are happy with what they have. rajakannu and sengeni plan a second child and soon sengeni gives the good news once rajkannu is called to the house of a upper caste man as a snake has sneaked inside his house.the next day theft of jewelry is reported in the same house suspicious raising towards rajkannu .the cops got to arrest rajkannu but he leaves the town for work following which the cops detain a pregnant sengani and rest of family members asking them details about the rajkannu.the cops trace rajkannu and torture him and his brothers in jail asking him to confess the crime they did not commit later sengeni finds that rajkannu and his brother have eloped from the prison to escape torture.mythra who teaches tribal village comes across a lawyer chandru who fights for tribal people and after hearing story of senegeni files a habeas corpus case in court.—alex.mjacko@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>227. Jai Bhim</t>
+          <t>227. Rush</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>rajakannu and his wife sengeni belong to a lower cast and works as labors in the field to protect it from rats thou they live life of poverty but are happy with what they have. rajakannu and sengeni plan a second child and soon sengeni gives the good news once rajkannu is called to the house of a upper caste man as a snake has sneaked inside his house.the next day theft of jewelry is reported in the same house suspicious raising towards rajkannu .the cops got to arrest rajkannu but he leaves the town for work following which the cops detain a pregnant sengani and rest of family members asking them details about the rajkannu.the cops trace rajkannu and torture him and his brothers in jail asking him to confess the crime they did not commit later sengeni finds that rajkannu and his brother have eloped from the prison to escape torture.mythra who teaches tribal village comes across a lawyer chandru who fights for tribal people and after hearing story of senegeni files a habeas corpus case in court.—alex.mjacko@gmail.com</t>
+          <t>set against the sexy, glamorous golden age of formula 1 racing in the 1970s, the film is based on the true story of a great sporting rivalry between handsome english playboy james hunt (hemsworth), and his methodical, brilliant opponent, austrian driver niki lauda (bruhl). the story follows their distinctly-different personal styles on and off the track, their loves, and the astonishing 1976 season in which both drivers were willing to risk everything to become world champion in a sport with no margin for error: if you make a mistake, you die.—p. morgan</t>
         </is>
       </c>
     </row>
@@ -3184,24 +3184,24 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>229. Stand by Me</t>
+          <t>229. The Wizard of Oz</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>it's the summer of 1959 in castlerock, oregon and four 12 year-old boys - gordie, chris, teddy and vern - are fast friends. after learning of the general location of the body of a local boy who has been missing for several days, they set off into the woods to see it. along the way, they learn about themselves, the meaning of friendship and the need to stand up for what is right.—garykmcd</t>
+          <t>when a tornado rips through kansas, dorothy gale and her dog, toto, are whisked away in their house to the magical land of oz. they follow the yellow brick road to the emerald city to meet the wizard, and on the way, they meet a scarecrow who wants a brain, a tin man who wants a heart, and a cowardly lion who wants courage. the wizard asks them to bring him the wicked witch of the west's broom to earn his help.—jwelch5742</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>230. The Wizard of Oz</t>
+          <t>230. Stand by Me</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>when a tornado rips through kansas, dorothy gale and her dog, toto, are whisked away in their house to the magical land of oz. they follow the yellow brick road to the emerald city to meet the wizard, and on the way, they meet a scarecrow who wants a brain, a tin man who wants a heart, and a cowardly lion who wants courage. the wizard asks them to bring him the wicked witch of the west's broom to earn his help.—jwelch5742</t>
+          <t>it's the summer of 1959 in castlerock, oregon and four 12 year-old boys - gordie, chris, teddy and vern - are fast friends. after learning of the general location of the body of a local boy who has been missing for several days, they set off into the woods to see it. along the way, they learn about themselves, the meaning of friendship and the need to stand up for what is right.—garykmcd</t>
         </is>
       </c>
     </row>
@@ -3232,36 +3232,36 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>233. Ah-ga-ssi</t>
+          <t>233. My Father and My Son</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>1930s korea, in the period of japanese occupation, a new girl (sookee) is hired as a handmaiden to a japanese heiress (hideko) who lives a secluded life on a large countryside estate with her domineering uncle (kouzuki). but the maid has a secret. she is a pickpocket recruited by a swindler posing as a japanese count to help him seduce the lady to elope with him, rob her of her fortune, and lock her up in a madhouse. the plan seems to proceed according to plan until sookee and hideko discover some unexpected emotions.—cj entertainment</t>
+          <t>sadik is one of the rebellious youth who has been politically active as a university student and became a left-wing journalist in the 70's, despite his father's expectations of him becoming an agricultural engineer and taking control of their family farm in an aegean village. on the dawn of september 12, 1980, when a merciless military coup hits the country, they cannot find access to any hospital or a doctor and his wife dies while giving birth to their only child, deniz. after a long-lasting period of torture, trials, and jail time, sadik returns to his village with 7-8 years old deniz, knowing that it will be hard to correct things with his father, huseyin.—ali riza bolukbasi</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>234. Into the Wild</t>
+          <t>234. The Handmaiden</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>based on a true story. after graduating from emory university, christopher mccandless abandoned his possessions, gave his entire savings account to charity, and hitchhiked to alaska to live in the wilderness. along the way, christopher encounters a series of characters who shape his life.—lisa kelley</t>
+          <t>1930s korea, in the period of japanese occupation, a new girl (sookee) is hired as a handmaiden to a japanese heiress (hideko) who lives a secluded life on a large countryside estate with her domineering uncle (kouzuki). but the maid has a secret. she is a pickpocket recruited by a swindler posing as a japanese count to help him seduce the lady to elope with him, rob her of her fortune, and lock her up in a madhouse. the plan seems to proceed according to plan until sookee and hideko discover some unexpected emotions.—cj entertainment</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>235. Babam ve Oglum</t>
+          <t>235. Into the Wild</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>sadik is one of the rebellious youth who has been politically active as a university student and became a left-wing journalist in the 70's, despite his father's expectations of him becoming an agricultural engineer and taking control of their family farm in an aegean village. on the dawn of september 12, 1980, when a merciless military coup hits the country, they cannot find access to any hospital or a doctor and his wife dies while giving birth to their only child, deniz. after a long-lasting period of torture, trials, and jail time, sadik returns to his village with 7-8 years old deniz, knowing that it will be hard to correct things with his father, huseyin.—ali riza bolukbasi</t>
+          <t>based on a true story. after graduating from emory university, christopher mccandless abandoned his possessions, gave his entire savings account to charity, and hitchhiked to alaska to live in the wilderness. along the way, christopher encounters a series of characters who shape his life.—lisa kelley</t>
         </is>
       </c>
     </row>
@@ -3280,24 +3280,24 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>237. La battaglia di Algeri</t>
+          <t>237. To Be or Not to Be</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>a film commissioned by the algerian government that shows the algerian revolution from both sides. the french foreign legion has left vietnam in defeat and has something to prove. the algerians are seeking independence. the two clash. the torture used by the french is contrasted with the algerian's use of bombs in soda shops. a look at war as a nasty thing that harms and sullies everyone who participates in it.—john vogel &lt;jlvogel@comcast.net&gt;</t>
+          <t>joseph and maria tura operate and star in their own theater company in warsaw. maria has many admirers including a young lieutenant in the polish air force, stanislav sobinski. when the germans invade poland to start world war ii, sobinski and his colleagues flee to england while the turas find themselves now having to operate under severe restrictions, including shelving a comical play they had written about adolf hitler. in england meanwhile, sobinski and his friends give professor siletski - who is about to return to poland - the names and addresses of their closest relatives so the professor can carry messages for them. when it's learned that siletski is really a german spy, sobinski parachutes into poland and enlists the aid of the turas and their fellow actors to get that list back.—garykmcd</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>238. To Be or Not to Be</t>
+          <t>238. The Battle of Algiers</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>joseph and maria tura operate and star in their own theater company in warsaw. maria has many admirers including a young lieutenant in the polish air force, stanislav sobinski. when the germans invade poland to start world war ii, sobinski and his colleagues flee to england while the turas find themselves now having to operate under severe restrictions, including shelving a comical play they had written about adolf hitler. in england meanwhile, sobinski and his friends give professor siletski - who is about to return to poland - the names and addresses of their closest relatives so the professor can carry messages for them. when it's learned that siletski is really a german spy, sobinski parachutes into poland and enlists the aid of the turas and their fellow actors to get that list back.—garykmcd</t>
+          <t>a film commissioned by the algerian government that shows the algerian revolution from both sides. the french foreign legion has left vietnam in defeat and has something to prove. the algerians are seeking independence. the two clash. the torture used by the french is contrasted with the algerian's use of bombs in soda shops. a look at war as a nasty thing that harms and sullies everyone who participates in it.—john vogel &lt;jlvogel@comcast.net&gt;</t>
         </is>
       </c>
     </row>
@@ -3328,7 +3328,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>241. Amores perros</t>
+          <t>241. Amores Perros</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -3340,24 +3340,24 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>242. The Iron Giant</t>
+          <t>242. Rebecca</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>this is the story of a nine-year-old boy named hogarth hughes who makes friends with an innocent alien giant robot that came from outer space. meanwhile, a paranoid u.s. government agent named kent mansley arrives in town, determined to destroy the giant at all costs. it's up to hogarth to protect him by keeping him at dean mccoppin's place in the junkyard.—anthony pereyra &lt;hypersonic91@yahoo.com&gt;</t>
+          <t>a shy lady's companion, staying in monte carlo with her stuffy employer, meets the wealthy maxim de winter (sir laurence olivier). she and max fall in love, marry, and return to manderley, his large country estate in cornwall. max is still troubled by the death of his first wife, rebecca, in a boating accident the year before. the second mrs. de winter (joan fontaine) clashes with the housekeeper, mrs. danvers (dame judith anderson), and discovers that rebecca still has a strange hold on everyone at manderley.—col needham &lt;col@imdb.com&gt;</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>243. Rebecca</t>
+          <t>243. The Iron Giant</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>a shy lady's companion, staying in monte carlo with her stuffy employer, meets the wealthy maxim de winter (sir laurence olivier). she and max fall in love, marry, and return to manderley, his large country estate in cornwall. max is still troubled by the death of his first wife, rebecca, in a boating accident the year before. the second mrs. de winter (joan fontaine) clashes with the housekeeper, mrs. danvers (dame judith anderson), and discovers that rebecca still has a strange hold on everyone at manderley.—col needham &lt;col@imdb.com&gt;</t>
+          <t>this is the story of a nine-year-old boy named hogarth hughes who makes friends with an innocent alien giant robot that came from outer space. meanwhile, a paranoid u.s. government agent named kent mansley arrives in town, determined to destroy the giant at all costs. it's up to hogarth to protect him by keeping him at dean mccoppin's place in the junkyard.—anthony pereyra &lt;hypersonic91@yahoo.com&gt;</t>
         </is>
       </c>
     </row>
@@ -3400,48 +3400,48 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>247. Dances with Wolves</t>
+          <t>247. Drishyam</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>lt. john dunbar is dubbed a hero after he accidentally leads union troops to a victory during the civil war. he requests a position on the western frontier, but finds it deserted. he soon finds out he is not alone, but meets a wolf he dubs "two-socks" and a curious sioux tribe. dunbar quickly makes friends with the tribe, and discovers a white woman who was raised by the sioux tribe. he gradually earns the respect of these native people, and they learn from each other and befriend each other.—greg bole &lt;bole@life.bio.sunysb.edu&gt;</t>
+          <t>vijay salgaonkar runs a cable tv network in a remote and hilly village of goa. he lives a happy life with his wife nandini and two daughters. a 4th grade dropout &amp; an orphan, vijay has worked his way towards success with his sheer hard-work &amp; street smartness in order to provide for his family who mean the world to him. a man of few means &amp; needs; vijay believes life is to be lived simplistically - his wife, while she loves him devoutly, wants vijay's thrifty &amp; miserly behavior to end and wants the world for her family. if there's one thing that vijay cannot live without, it is his passion for watching films. such is his 'filmy' obsession that he doesn't mind staying up all night at his office binging on tv movies! in a bizarre turn of events; a teenage boy goes missing; he is the son of a headstrong &amp; no-nonsense cop; ig meera deshmukh and the salgaonkar family is the prime suspect! will a humble &amp; middle class man, be able to protect his family from oppression of the powerful? how the family weathers the storm that ensues during the violent investigation forms the rest of the story leading to an unexpected &amp; shocking climax.—dhruvi dokania</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>248. Aladdin</t>
+          <t>248. Gangs of Wasseypur</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>aladdin is a poor street urchin who spends his time stealing food from the marketplace in the city of agrabah. his adventures begin when he meets a young girl who happens to be princess jasmine, whose wacky, estranged father is forcing her to get married. aladdin's luck suddenly changes when he retrieves a magical lamp from the cave of wonders. what he unwittingly gets is a fun-loving genie who only wishes to have his freedom. little do they know that the sultan's sinister advisor jafar has his own plans for both aladdin and the lamp.—blazer346</t>
+          <t>shahid khan is exiled after impersonating the legendary sultana daku in order to rob british trains. now outcast, shahid becomes a worker at ramadhir singh's colliery, only to spur a revenge battle that passes on to generations. at the turn of the decade, shahid's son, the philandering sardar khan vows to get his father's honor back, becoming the most feared man of wasseypur.—anonymous</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>249. Drishyam</t>
+          <t>249. Dances with Wolves</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>vijay salgaonkar runs a cable tv network in a remote and hilly village of goa. he lives a happy life with his wife nandini and two daughters. a 4th grade dropout &amp; an orphan, vijay has worked his way towards success with his sheer hard-work &amp; street smartness in order to provide for his family who mean the world to him. a man of few means &amp; needs; vijay believes life is to be lived simplistically - his wife, while she loves him devoutly, wants vijay's thrifty &amp; miserly behavior to end and wants the world for her family. if there's one thing that vijay cannot live without, it is his passion for watching films. such is his 'filmy' obsession that he doesn't mind staying up all night at his office binging on tv movies! in a bizarre turn of events; a teenage boy goes missing; he is the son of a headstrong &amp; no-nonsense cop; ig meera deshmukh and the salgaonkar family is the prime suspect! will a humble &amp; middle class man, be able to protect his family from oppression of the powerful? how the family weathers the storm that ensues during the violent investigation forms the rest of the story leading to an unexpected &amp; shocking climax.—dhruvi dokania</t>
+          <t>lt. john dunbar is dubbed a hero after he accidentally leads union troops to a victory during the civil war. he requests a position on the western frontier, but finds it deserted. he soon finds out he is not alone, but meets a wolf he dubs "two-socks" and a curious sioux tribe. dunbar quickly makes friends with the tribe, and discovers a white woman who was raised by the sioux tribe. he gradually earns the respect of these native people, and they learn from each other and befriend each other.—greg bole &lt;bole@life.bio.sunysb.edu&gt;</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>250. Gangs of Wasseypur</t>
+          <t>250. Aladdin</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>shahid khan is exiled after impersonating the legendary sultana daku in order to rob british trains. now outcast, shahid becomes a worker at ramadhir singh's colliery, only to spur a revenge battle that passes on to generations. at the turn of the decade, shahid's son, the philandering sardar khan vows to get his father's honor back, becoming the most feared man of wasseypur.—anonymous</t>
+          <t>aladdin is a poor street urchin who spends his time stealing food from the marketplace in the city of agrabah. his adventures begin when he meets a young girl who happens to be princess jasmine, whose wacky, estranged father is forcing her to get married. aladdin's luck suddenly changes when he retrieves a magical lamp from the cave of wonders. what he unwittingly gets is a fun-loving genie who only wishes to have his freedom. little do they know that the sultan's sinister advisor jafar has his own plans for both aladdin and the lamp.—blazer346</t>
         </is>
       </c>
     </row>

</xml_diff>